<commit_message>
changed Preis 2 to Preis 1
</commit_message>
<xml_diff>
--- a/vormonat/KO_Verrechnung_CeBrACloudServer_intern_OK.xlsx
+++ b/vormonat/KO_Verrechnung_CeBrACloudServer_intern_OK.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\TI230\DSIM-CCS\02 ADMINISTRATION\Verrechnung\2020-03\KO\dummy_vorquartal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\TI230\DSIM-CCS\02 ADMINISTRATION\Verrechnung\2020-03\KO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B1CCED-4254-44F2-9C39-A62C54CFC2A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775D8639-2F99-40A9-A88B-963F2A04A533}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1605" windowWidth="19200" windowHeight="16830" xr2:uid="{8E88CE84-CBA6-4CBC-B0FA-B299D8A4D79D}"/>
+    <workbookView xWindow="0" yWindow="1605" windowWidth="19200" windowHeight="16830" firstSheet="4" activeTab="8" xr2:uid="{8E88CE84-CBA6-4CBC-B0FA-B299D8A4D79D}"/>
   </bookViews>
   <sheets>
     <sheet name="SMS" sheetId="10" r:id="rId1"/>
@@ -7241,8 +7241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71451CB6-1B52-4444-9245-704BE73886F4}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7313,7 +7313,7 @@
         <v>2277</v>
       </c>
       <c r="G3">
-        <v>1215</v>
+        <v>458.4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -7349,7 +7349,7 @@
   <dimension ref="A1:G706"/>
   <sheetViews>
     <sheetView topLeftCell="A680" workbookViewId="0">
-      <selection activeCell="G690" sqref="G690"/>
+      <selection activeCell="D716" sqref="D716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23198,7 +23198,7 @@
         <v>14</v>
       </c>
       <c r="G689">
-        <v>544857</v>
+        <v>900</v>
       </c>
     </row>
     <row r="690" spans="1:7" x14ac:dyDescent="0.25">
@@ -23602,7 +23602,7 @@
   <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25720,7 +25720,7 @@
         <v>14</v>
       </c>
       <c r="G92">
-        <v>65468</v>
+        <v>3459</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -25904,7 +25904,7 @@
         <v>14</v>
       </c>
       <c r="G100">
-        <v>9887</v>
+        <v>900</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -25963,7 +25963,7 @@
   <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G102" sqref="G102"/>
+      <selection activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28288,7 +28288,7 @@
         <v>14</v>
       </c>
       <c r="G101">
-        <v>456274</v>
+        <v>677.09999999999991</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -28416,7 +28416,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28625,7 +28625,7 @@
         <v>14</v>
       </c>
       <c r="G9">
-        <v>42</v>
+        <v>374.4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -31091,7 +31091,7 @@
   <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="I90" sqref="I90"/>
+      <selection activeCell="G106" sqref="G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33163,7 +33163,7 @@
         <v>14</v>
       </c>
       <c r="G90">
-        <v>22</v>
+        <v>1.2000000000000002</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -33521,7 +33521,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33592,7 +33592,7 @@
         <v>14</v>
       </c>
       <c r="G3">
-        <v>4526</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -33627,8 +33627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418A3890-34B3-42A4-BA5A-CE4A41DDE108}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33837,7 +33837,7 @@
         <v>14</v>
       </c>
       <c r="G9">
-        <v>16874</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>